<commit_message>
UI：Able to update according to inventory
</commit_message>
<xml_diff>
--- a/Assets/Editor/ItemTree.xlsx
+++ b/Assets/Editor/ItemTree.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhuguan\Documents\GitHub\sprint01-factory-prototype\Assets\Editor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习\Sheridan\Year2\Y2S2\DesignPractice\FactoryGame\sprint01-factory-prototype\Assets\Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8DCFCD-6BB7-4334-88CA-07B8473176AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9F33B7-924E-40B0-A339-BEFD1EB84D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1470" windowWidth="17100" windowHeight="11880" xr2:uid="{6A58C925-9F2D-4C6C-91BC-1ECBCC8690DD}"/>
+    <workbookView xWindow="9886" yWindow="2481" windowWidth="17147" windowHeight="10152" xr2:uid="{6A58C925-9F2D-4C6C-91BC-1ECBCC8690DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Items</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,24 +94,28 @@
   </si>
   <si>
     <t>Sand</t>
+  </si>
+  <si>
+    <t>Mushroom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -120,7 +124,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -194,8 +198,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26679EAA-8BFE-48F6-A2D8-A3369DDEB193}" name="Items" displayName="Items" ref="B3:G12" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:G12" xr:uid="{26679EAA-8BFE-48F6-A2D8-A3369DDEB193}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26679EAA-8BFE-48F6-A2D8-A3369DDEB193}" name="Items" displayName="Items" ref="B3:G13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:G13" xr:uid="{26679EAA-8BFE-48F6-A2D8-A3369DDEB193}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6F7920FD-881E-4ACC-B371-596C4C5A23D8}" name="Name"/>
     <tableColumn id="2" xr3:uid="{81785AEB-273F-45A0-A058-30B3A5C50566}" name="Tier"/>
@@ -525,27 +529,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CBD926-4FFC-43C9-8374-F00B833293BB}">
-  <dimension ref="B2:I12"/>
+  <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -567,7 +571,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -575,7 +579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -583,7 +587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -591,7 +595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -599,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -619,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -639,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -659,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -679,7 +683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -697,6 +701,26 @@
       </c>
       <c r="G12">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>